<commit_message>
update excel ( add float )
</commit_message>
<xml_diff>
--- a/test/support/spreadsheet/utf8.xlsx
+++ b/test/support/spreadsheet/utf8.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F0671A1-8A84-4CB7-9575-E687FC4367B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24980610-CE8E-4B67-B0B6-B821028B406A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>姓名</t>
   </si>
   <si>
     <t>電話</t>
+  </si>
+  <si>
+    <t>pi</t>
   </si>
   <si>
     <t>許功蓋</t>
@@ -390,31 +393,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3.1415926535900001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>